<commit_message>
update UAT test version 2
</commit_message>
<xml_diff>
--- a/Project/sprint02/UAT_Sprint2.xlsx
+++ b/Project/sprint02/UAT_Sprint2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/puriwatsreprach/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/puriwatsreprach/Github/Software-Engineer-group5/Project/sprint02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{219F7AC9-856B-4242-96AF-4D14A1FF019F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA96429-C811-2642-8A4A-293FD204F322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>EC-Lab10</t>
   </si>
@@ -97,9 +97,6 @@
 1. คลิกที่ไอคอน : 'English flag'</t>
   </si>
   <si>
-    <t xml:space="preserve">ภาษาของหน้าเว็บไซต์เปลี่ยนเป็นภาษาอังกฤษ และแสดงปุ่มธงชาติไทย อังกฤษ และอิโดนีเซียตามลำดับ  </t>
-  </si>
-  <si>
     <t>TC16_03</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
 1. คลิกที่ไอคอน : 'Indonesia flag'</t>
   </si>
   <si>
-    <t xml:space="preserve">ภาษาของหน้าเว็บไซต์เปลี่ยนเป็นภาษาอินโดนีเซีย และแสดงปุ่มธงชาติไทย อังกฤษ และอิโดนีเซียตามลำดับ  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">เปลี่ยนภาษาของหน้าเว็บไซต์เป็นภาษาอินโดนีเซียและเปลี่ยนปุ่มธงชาติเป็นธงชาติไทย  </t>
-  </si>
-  <si>
     <t>TC16_04</t>
   </si>
   <si>
@@ -122,62 +113,126 @@
 1. คลิกที่ไอคอน : 'Thai flag'  </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>แสดงหน้าแรกของเว็บไซต์เป็นภาษาไทย และแสดงปุ่มธงชาติอังกฤษ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>TC16_05</t>
   </si>
   <si>
-    <t xml:space="preserve">TC05
-ที่หน้า Home :
-1. คลิกที่ไอคอน : 'ธงชาติไทย'  </t>
-  </si>
-  <si>
     <t>TC16_06</t>
   </si>
   <si>
-    <t xml:space="preserve">TC06
-ที่หน้า Home :
-1. คลิกที่ไอคอน : 'ธงชาติไทย'  </t>
-  </si>
-  <si>
     <t>TC16_07</t>
   </si>
   <si>
-    <t xml:space="preserve">TC07
-ที่หน้า Home :
-1. คลิกที่ไอคอน : 'ธงชาติไทย'  </t>
-  </si>
-  <si>
     <t>TC16_08</t>
   </si>
   <si>
-    <t xml:space="preserve">TC08
-ที่หน้า Home :
-1. คลิกที่ไอคอน : 'ธงชาติไทย'  </t>
+    <t>หน้าเว็บแสดงข้อความ สินค้ายอดนิยม
+แสดงชื่อสินค้าเป็นแก้วเก็บความเย็น</t>
+  </si>
+  <si>
+    <t>หน้าเว็บแสดงข้อความ Popular Products แสดงชื่อสินค้าเป็น cold glass</t>
+  </si>
+  <si>
+    <t>หน้าเว็บแสดงข้อความ Populer แสดงชื่อสินค้าเป็น gelas dingin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC11
+1.เลือกรายการสินค้า เสื้อโปโล วิทยาลัยการคอมพิวเตอร์
+2. ขวดน้ำ CP
+3. คลิกที่ไอคอน : 'อังกฤษ'
+</t>
+  </si>
+  <si>
+    <t>แสดงรายละเอียดสินค้าและชื่อเป็น เสื้อโปโล วิทยาลัยการคอมพิวเตอร์ จากนั้นแสดงรายการสินค้าชื่อ  ขวดน้ำ CP เมื่อเปลี่ยนเป็นภาษา อังกฤษ จะแสดงชื่อสินค้าเป็น CP water bottle</t>
+  </si>
+  <si>
+    <t>แสดงรายละเอียดสินค้าและชื่อเป็น ceramic mug  เมื่อเปลี่ยนเป็นภาษา อินโดนีเซีย จะแสดงชื่อสินค้าเป็น Cangkir keramik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC11
+1.เลือกรายการสินค้า ceramic mug 
+2. ขวดน้ำ CP
+3. คลิกที่ไอคอน : 'อังกฤษ'
+</t>
+  </si>
+  <si>
+    <t>in homepage :
+1. คลิกที่ไอคอน : 'ธงชาติไทย'  
+2.เลือกรายการสินค้า แก้วเก็บความเย็น</t>
+  </si>
+  <si>
+    <t>in homepage :
+1. คลิกที่ไอคอน : 'อังกฤษ'  
+2.เลือกรายการสินค้า แก้วเก็บความเย็น</t>
+  </si>
+  <si>
+    <t>in homepage :
+1.คลิกที่ไอคอน:'ธงชาติอินโด'
+2.เลือกรายการสินค้า แก้วเก็บความเย็น</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add product in thai :
+in home page : 
+1. เลือกที่ ขวดน้ำ CP
+2. คลิกที่ หยิบใส่ตะกร้า
+3. คลิกที่ ทำรายการชำระเงิน
+4. คลิกที่ ทำรายการชำระเงิน อีกครั้ง
+</t>
+  </si>
+  <si>
+    <t>แสดงหน้าแรกเป็นภาษาไทย จากนั้นแสดงหน้ารายละเอียดสินค้า ขวดน้ำ CP เมือกด ทำรายการชำระเงิน จะแสดงหน้า ตะกร้าสินค้า และแสดงหน้า ข้อมูลส่วนตัว</t>
+  </si>
+  <si>
+    <t>แสดงหน้าแรกเป็นภาษาอังกฤษ จากนั้นแสดงหน้ารายละเอียดสินค้า CP water bottle เมือกด ทำรายการชำระเงิน จะแสดงหน้า Shopping Cart และแสดงหน้า Personal Information</t>
+  </si>
+  <si>
+    <t>in home page :
+1. เลือกที่ CP water bottle
+2. คลิกที่  Add to car
+3. คลิกที่ Proceed to checkout
+4. คลิกที่ Proceed to checkou อีกครั้ง</t>
+  </si>
+  <si>
+    <t>in home page :
+1. เลือกที่ Botol air CP
+2. คลิกที่  Bel
+3. คลิกที่  Proses pembayaran
+4. คลิกที่  Proses pembayaran อีกครั้ง</t>
+  </si>
+  <si>
+    <t>แสดงหน้าแรกเป็นภาษาอังกฤษ จากนั้นแสดงหน้ารายละเอียดสินค้า Botol air CP เมือกด ทำรายการชำระเงิน จะแสดงหน้า Troli Belanja และแสดงหน้า Informasi Anda</t>
+  </si>
+  <si>
+    <t>แสดงหน้าแรกเป็นภาษาไทย แสดงหมวดหมู่ เสื้อผ้า และแสดงหมวดย่อยเป็น ผู้ชาย ผู้หญิง</t>
+  </si>
+  <si>
+    <t>Category Cloth thia
+in homepage :
+1. เลือกที่หมวดหมู่ เสื้อผ้า</t>
+  </si>
+  <si>
+    <t>in homepage :
+1. เลือกที่หมวดหมู่  เสื้อผ้า
+2. เลือกเปี่ยนภาษาเป็น อังกฤษ</t>
+  </si>
+  <si>
+    <t>in homepage :
+1. เลือกที่หมวดหมู่  เสื้อผ้า
+2. เลือกเปี่ยนภาษาเป็น อินโดนีเซีย</t>
+  </si>
+  <si>
+    <t>แสดงหน้าแรกเป็นภาษาไทย แสดงหมวดหมู่ เสื้อผ้า เป็นภาษาอังกฤษ Clothes และแสดงหมวดย่อยเป็น Men Women</t>
+  </si>
+  <si>
+    <t>แสดงหน้าแรกเป็นภาษาไทย แสดงหมวดหมู่ เสื้อผ้า เป็นภาษาอินโดนีเซีย Pakaian และแสดงหมวดย่อยเป็น Pria Wanita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ภาษาของหน้าเว็บไซต์เปลี่ยนเป็นภาษาอังกฤษ แสดงข้อความ Popular Products และแสดงปุ่มธงชาติ อังกฤษ ไทย และอิโดนีเซียตามลำดับ  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ภาษาของหน้าเว็บไซต์เปลี่ยนเป็นภาษาอินโดนีเซีย แสดงข้อความ Populer และแสดงปุ่มธงชาติ อังกฤษ ไทย และอิโดนีเซียตามลำดับ  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">แสดงหน้าแรกของเว็บไซต์เป็นภาษาไทย แสดงข้อความ สินค้ายอดนิยม และแสดงปุ่มธงชาติ อังกฤษ ไทย และอิโดนีเซียตามลำดับ  </t>
   </si>
 </sst>
 </file>
@@ -187,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +295,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -265,17 +326,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -358,74 +408,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -658,409 +730,475 @@
     <col min="7" max="26" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="14">
         <v>24778</v>
       </c>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="17"/>
-    </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="8" t="s">
+      <c r="E9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="8" t="s">
+      <c r="C11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C12" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D12" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="8" t="s">
+      <c r="C13" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="C15" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="102" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="C16" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" ht="51" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="8" t="s">
+      <c r="D16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E17" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="28"/>
+    </row>
+    <row r="21" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" spans="1:6" ht="101" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="28"/>
+    </row>
+    <row r="24" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2026,7 +2164,6 @@
   <mergeCells count="10">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A9:A16"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
@@ -2034,6 +2171,7 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="A9:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>